<commit_message>
Ändrat namn på excelfilerna så jag vet vilka jag gjort själv. Gjort en vettig framstegsöversikt.
</commit_message>
<xml_diff>
--- a/Rawdata/metadataframsteg.xlsx
+++ b/Rawdata/metadataframsteg.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14120" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
+    <workbookView xWindow="460" yWindow="1200" windowWidth="25440" windowHeight="11340" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>Moment</t>
   </si>
@@ -32,32 +32,122 @@
     <t>status</t>
   </si>
   <si>
-    <t>data ripinventering omgång 1</t>
-  </si>
-  <si>
     <t>klar</t>
   </si>
   <si>
-    <t>data ripinventering omgång 2</t>
-  </si>
-  <si>
-    <t>lydata omgång 1</t>
-  </si>
-  <si>
-    <t>lyaktivitet vår</t>
-  </si>
-  <si>
     <t>lyaktivitet reproduktion</t>
+  </si>
+  <si>
+    <t>lyaktivitet vår rovbase</t>
+  </si>
+  <si>
+    <t>kommentar</t>
+  </si>
+  <si>
+    <t>påbörjat</t>
+  </si>
+  <si>
+    <t>klart för de ripinventerade lyorna, kanske måste ha hjälp med ett r-skript för att automatisera avstånd till trädgränsen för resten av lyorna?</t>
+  </si>
+  <si>
+    <t>klart för de ripinventerade lyorna, kanske måste ha hjälp med ett r-skript för att automatisera avstånd till vatten för resten av lyorna?</t>
+  </si>
+  <si>
+    <t>ej påbörjat</t>
+  </si>
+  <si>
+    <t>hur göra detta? Det rimliga vore avstånd till andra aktiva lyor. Detta kommer alltså att ändras från år till år. Hur gör jag det i r?</t>
+  </si>
+  <si>
+    <t>hur göra detta? Det rimliga vore avstånd till  aktiva rödrävslyor från varje aktiv fjällrävslya. Detta kommer alltså att ändras från år till år. Hur gör jag det i r?</t>
+  </si>
+  <si>
+    <t>mata in data ripinventering omgång 1</t>
+  </si>
+  <si>
+    <t>mata in data ripinventering omgång 2</t>
+  </si>
+  <si>
+    <t>mata in lydata (snötäcke, marktemp etc.) omgång 1</t>
+  </si>
+  <si>
+    <t>mata in lydata (snötäcke, marktemp etc.) omgång 2</t>
+  </si>
+  <si>
+    <t>finns tyvärr ej lagrat i gps.</t>
+  </si>
+  <si>
+    <t>GIS-data lyornas höjd över havet</t>
+  </si>
+  <si>
+    <t>GIS-data lyornas avstånd andra fjällrävslyor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIS-data lyornas avstånd vattendrag eller sjöar </t>
+  </si>
+  <si>
+    <t>GIS-data lyornas avstånd trädgräns</t>
+  </si>
+  <si>
+    <t>GIS-data lyornas avstånd till rödrävslyor</t>
+  </si>
+  <si>
+    <t>Helinventeringar gnagare</t>
+  </si>
+  <si>
+    <t>Helinventeringar fågel</t>
+  </si>
+  <si>
+    <t>Sannolikhet för lämmel inom x radie från lyan</t>
+  </si>
+  <si>
+    <t>lyaktivitet vår, Lars data</t>
+  </si>
+  <si>
+    <t>fått "lemming-index" av Rasmus, vad exakt anger det? Ska jag använda "sannolikhet för lämmel - modellen" inom hela området eller ta andel bra lämmelhabitat och sätta ett gränsvärde?</t>
+  </si>
+  <si>
+    <t>mailat Lars men ej fått svar, ring i morgon</t>
+  </si>
+  <si>
+    <t>fått datan av Rasmus. Betyder "Komplexbin = 1" att det var två kullar i lyan?</t>
+  </si>
+  <si>
+    <t>Helinventeringar växtkartering</t>
+  </si>
+  <si>
+    <t>Behöver jag den här? Kanske onödig</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -83,8 +173,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,51 +492,182 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B3727A8-9212-7041-83C2-501947B2BAAE}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="46.83203125" customWidth="1"/>
+    <col min="3" max="3" width="132.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Höjddata för Helagslyorna inlagda i ett separat dokument. inga större ändringar i R-skript.
</commit_message>
<xml_diff>
--- a/Rawdata/metadataframsteg.xlsx
+++ b/Rawdata/metadataframsteg.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="460" yWindow="1200" windowWidth="25440" windowHeight="11340" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
+    <workbookView xWindow="160" yWindow="1420" windowWidth="25440" windowHeight="11340" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>Moment</t>
   </si>
@@ -74,9 +74,6 @@
     <t>mata in lydata (snötäcke, marktemp etc.) omgång 2</t>
   </si>
   <si>
-    <t>finns tyvärr ej lagrat i gps.</t>
-  </si>
-  <si>
     <t>GIS-data lyornas höjd över havet</t>
   </si>
   <si>
@@ -104,26 +101,26 @@
     <t>lyaktivitet vår, Lars data</t>
   </si>
   <si>
-    <t>fått "lemming-index" av Rasmus, vad exakt anger det? Ska jag använda "sannolikhet för lämmel - modellen" inom hela området eller ta andel bra lämmelhabitat och sätta ett gränsvärde?</t>
-  </si>
-  <si>
-    <t>mailat Lars men ej fått svar, ring i morgon</t>
-  </si>
-  <si>
-    <t>fått datan av Rasmus. Betyder "Komplexbin = 1" att det var två kullar i lyan?</t>
-  </si>
-  <si>
     <t>Helinventeringar växtkartering</t>
   </si>
   <si>
     <t>Behöver jag den här? Kanske onödig</t>
+  </si>
+  <si>
+    <t>fått datan av Rasmus. Gjort en separat fil för de ripinventerade lyorna, dock verkar det saknas data för "2003", "2006", "2009", "2012", "2016". 2016 fanns i rovbase</t>
+  </si>
+  <si>
+    <t>Andel bra lämmelhabitat inom området (sätt gränsvärde)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lars skulle se vad han hade. Han har mailat en del data tidigare år (c:a 2000 - 2005)  till Tomas Meijer och kanske till Anders. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -152,6 +149,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri (Brödtext)_x0000_"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -173,11 +175,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,19 +495,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B3727A8-9212-7041-83C2-501947B2BAAE}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="46.83203125" customWidth="1"/>
     <col min="3" max="3" width="132.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -515,7 +518,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -523,7 +526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -531,7 +534,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -539,7 +542,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -547,7 +550,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -555,18 +558,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -574,12 +577,12 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>6</v>
@@ -588,9 +591,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>6</v>
@@ -599,9 +602,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>9</v>
@@ -610,9 +613,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>9</v>
@@ -621,53 +624,55 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" customHeight="1">
+      <c r="A15" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="B15" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15" customHeight="1">
+      <c r="A17" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>24</v>
-      </c>
       <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C17" t="s">
-        <v>26</v>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lagt till tankar om bra lämmelhabitat.
</commit_message>
<xml_diff>
--- a/Rawdata/metadataframsteg.xlsx
+++ b/Rawdata/metadataframsteg.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="160" yWindow="1420" windowWidth="25440" windowHeight="11340" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
+    <workbookView xWindow="160" yWindow="1740" windowWidth="25440" windowHeight="11340" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>Moment</t>
   </si>
@@ -95,25 +95,31 @@
     <t>Helinventeringar fågel</t>
   </si>
   <si>
-    <t>Sannolikhet för lämmel inom x radie från lyan</t>
-  </si>
-  <si>
     <t>lyaktivitet vår, Lars data</t>
   </si>
   <si>
     <t>Helinventeringar växtkartering</t>
   </si>
   <si>
-    <t>Behöver jag den här? Kanske onödig</t>
-  </si>
-  <si>
     <t>fått datan av Rasmus. Gjort en separat fil för de ripinventerade lyorna, dock verkar det saknas data för "2003", "2006", "2009", "2012", "2016". 2016 fanns i rovbase</t>
   </si>
   <si>
-    <t>Andel bra lämmelhabitat inom området (sätt gränsvärde)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lars skulle se vad han hade. Han har mailat en del data tidigare år (c:a 2000 - 2005)  till Tomas Meijer och kanske till Anders. </t>
+  </si>
+  <si>
+    <t>Behöver jag den här? Kanske onödig. Får se vad NDVI säger först.</t>
+  </si>
+  <si>
+    <t>Sannolikhet för lämmel inom riptriangeln runt lyan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iptrianglarna eftersom rävar jagar närmare lyan när de har valpar (Frafjord 1993) och måste bära tillbaka mat till lyan (Zapata et al. 1998. Dessutom måste jag hålla observationerna oberoende av varandra. Gallant et al (2014) valde max radius på 1,5 km. </t>
+  </si>
+  <si>
+    <t>Andel bra lämmelhabitat inom området (sätt gränsvärde för lämmelsannolikhet per pixel)</t>
+  </si>
+  <si>
+    <t>Vad är det maximala sannolikhetsvärdet i en pixel för lämmel under uppgångsfas? I så fall kan jag ta hälften av det som gränsvärde för bra lämmelhabitat.</t>
   </si>
 </sst>
 </file>
@@ -498,7 +504,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -560,13 +566,13 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -577,7 +583,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -650,29 +656,35 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15" customHeight="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" customHeight="1">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
påbörjat skript för avstånd till vatten och skog. Har sammanfogat shapefilerna för små och stora vatten. En för norra delen och en för södra delen. Har dock inte lyckats sammanfoga de två nya shapefilerna. Nu har jag en komplett för norr och en komplett för söder. Har ingen karta över norsk skog än.
</commit_message>
<xml_diff>
--- a/Rawdata/metadataframsteg.xlsx
+++ b/Rawdata/metadataframsteg.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="160" yWindow="1740" windowWidth="25440" windowHeight="11340" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
+    <workbookView xWindow="160" yWindow="900" windowWidth="25440" windowHeight="11340" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -59,9 +59,6 @@
     <t>hur göra detta? Det rimliga vore avstånd till andra aktiva lyor. Detta kommer alltså att ändras från år till år. Hur gör jag det i r?</t>
   </si>
   <si>
-    <t>hur göra detta? Det rimliga vore avstånd till  aktiva rödrävslyor från varje aktiv fjällrävslya. Detta kommer alltså att ändras från år till år. Hur gör jag det i r?</t>
-  </si>
-  <si>
     <t>mata in data ripinventering omgång 1</t>
   </si>
   <si>
@@ -120,6 +117,9 @@
   </si>
   <si>
     <t>Vad är det maximala sannolikhetsvärdet i en pixel för lämmel under uppgångsfas? I så fall kan jag ta hälften av det som gränsvärde för bra lämmelhabitat.</t>
+  </si>
+  <si>
+    <t>verkar som att det finns rödrävsdata i Peters fil fram till 2008 (röd text). hur göra detta? Det rimliga vore avstånd till  aktiva rödrävslyor från varje aktiv fjällrävslya. Detta kommer alltså att ändras från år till år. Hur gör jag det i r?</t>
   </si>
 </sst>
 </file>
@@ -504,7 +504,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -526,7 +526,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -534,7 +534,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
@@ -550,7 +550,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
@@ -566,13 +566,13 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -583,12 +583,12 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>6</v>
@@ -599,7 +599,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>6</v>
@@ -610,7 +610,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>9</v>
@@ -621,18 +621,18 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>2</v>
@@ -640,7 +640,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>9</v>
@@ -648,7 +648,7 @@
     </row>
     <row r="15" spans="1:3" ht="15" customHeight="1">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>9</v>
@@ -656,35 +656,35 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1">
       <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
         <v>28</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
         <v>30</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lagt till avstånd från lyor till vatten och lyor till skog (utan gps-punkter). Bytt namn på filen med avståndet som är mätta för hand från de ripinventerade lyorna.
</commit_message>
<xml_diff>
--- a/Rawdata/metadataframsteg.xlsx
+++ b/Rawdata/metadataframsteg.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="160" yWindow="900" windowWidth="25440" windowHeight="11340" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
+    <workbookView xWindow="560" yWindow="3480" windowWidth="25440" windowHeight="11340" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -503,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B3727A8-9212-7041-83C2-501947B2BAAE}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
uppdaterat framstegmetadata och lagt till avstånd till vatten och skog som en separat excel-fil.
</commit_message>
<xml_diff>
--- a/Rawdata/metadataframsteg.xlsx
+++ b/Rawdata/metadataframsteg.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="560" yWindow="3480" windowWidth="25440" windowHeight="11340" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
+    <workbookView xWindow="160" yWindow="3200" windowWidth="25440" windowHeight="11340" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -104,22 +104,22 @@
     <t>Andel bra lämmelhabitat inom området (sätt gränsvärde för lämmelsannolikhet per pixel)</t>
   </si>
   <si>
-    <t>Vad är det maximala sannolikhetsvärdet i en pixel för lämmel under uppgångsfas? I så fall kan jag ta hälften av det som gränsvärde för bra lämmelhabitat.</t>
-  </si>
-  <si>
     <t>tog bort små trädsamlingar som inte satt ihop med skog som går ner i låglandet.</t>
   </si>
   <si>
-    <t>klart för de ripinventerade lyorna, klart för närmsta vattenkälla. Måste ta avstånd till större vatten. Bestäm ett gränsvärde (m^2), lägg till i attributes och ta bort.</t>
-  </si>
-  <si>
     <t>fått datan av Rasmus. Gjort en separat fil för de ripinventerade lyorna, dock verkar det saknas data för "2003", "2006", "2009", "2012", "2016". 2016 tog jag ur rovbase. 2012 var det inga. 2009 var det två (vilka). 2003 och 2006 finns i Peters fil.</t>
   </si>
   <si>
-    <t>hur göra detta? Det rimliga vore avstånd till andra aktiva lyor. Detta kommer alltså att ändras från år till år. Fått skript av Rasmus?</t>
-  </si>
-  <si>
     <t xml:space="preserve">det finns rödrävsreproduktion i Peters fil fram till 2008 (röd text) dock är det bara två totalt. Använd koordinaterna för skjutna rävar istället.  Använd Rasmus skript. </t>
+  </si>
+  <si>
+    <t>klart för de ripinventerade lyorna, klart för närmsta vattenkälla för alla lyor. Måste ta avstånd till större vatten. Bestäm ett gränsvärde (m^2), lägg till i attributes och ta bort.</t>
+  </si>
+  <si>
+    <t>Fått skript av Rasmus, ändra om till mina data.</t>
+  </si>
+  <si>
+    <t>Den högsta sannolikheten för lämmel i en 500 x 500 m pixel är 0,4 under ett uppgångsår. Jag räknar allt från 0,2 och över som bra lämmelhabitat. Toppåren är inte lika intressanta eftersom lämlarna finns överallt.</t>
   </si>
 </sst>
 </file>
@@ -504,7 +504,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -583,7 +583,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -594,7 +594,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -605,7 +605,7 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -627,7 +627,7 @@
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -684,7 +684,7 @@
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
några ändringar i avstånd närmsta aktiva lya(flyttat en del filer så de måste läsas in igen). ändrat i metadataframsteg. Lagt till ett skript för att få ut lyor med reproduktion ur Alvas data (RelevantEvents). Det funkade inte så bra då det fattas datum för många obsar.Börjat mata in sommarens riptransekter
</commit_message>
<xml_diff>
--- a/Rawdata/metadataframsteg.xlsx
+++ b/Rawdata/metadataframsteg.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="160" yWindow="3200" windowWidth="25440" windowHeight="11340" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
+    <workbookView xWindow="-360" yWindow="5620" windowWidth="25440" windowHeight="11340" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -89,9 +89,6 @@
     <t>Helinventeringar växtkartering</t>
   </si>
   <si>
-    <t xml:space="preserve">Lars skulle se vad han hade. Han har mailat en del data tidigare år (c:a 2000 - 2005)  till Tomas Meijer och kanske till Anders. </t>
-  </si>
-  <si>
     <t>Behöver jag den här? Kanske onödig. Får se vad NDVI säger först.</t>
   </si>
   <si>
@@ -107,26 +104,29 @@
     <t>tog bort små trädsamlingar som inte satt ihop med skog som går ner i låglandet.</t>
   </si>
   <si>
-    <t>fått datan av Rasmus. Gjort en separat fil för de ripinventerade lyorna, dock verkar det saknas data för "2003", "2006", "2009", "2012", "2016". 2016 tog jag ur rovbase. 2012 var det inga. 2009 var det två (vilka). 2003 och 2006 finns i Peters fil.</t>
-  </si>
-  <si>
     <t xml:space="preserve">det finns rödrävsreproduktion i Peters fil fram till 2008 (röd text) dock är det bara två totalt. Använd koordinaterna för skjutna rävar istället.  Använd Rasmus skript. </t>
   </si>
   <si>
     <t>klart för de ripinventerade lyorna, klart för närmsta vattenkälla för alla lyor. Måste ta avstånd till större vatten. Bestäm ett gränsvärde (m^2), lägg till i attributes och ta bort.</t>
   </si>
   <si>
-    <t>Fått skript av Rasmus, ändra om till mina data.</t>
-  </si>
-  <si>
     <t>Den högsta sannolikheten för lämmel i en 500 x 500 m pixel är 0,4 under ett uppgångsår. Jag räknar allt från 0,2 och över som bra lämmelhabitat. Toppåren är inte lika intressanta eftersom lämlarna finns överallt.</t>
+  </si>
+  <si>
+    <t>Fått skript av Rasmus, ändra om till mina data. Fattas för vissa år i Rasmus.kulldata till Tor och i Lypositioner kullar 2000-2017 SWEREF99 per kull (finns mer data i den senare även fast Rasmus tagit bort lågår och omatade lyor. Komplettera med data från filen Red fox feeding och hitta vilka två lyor det var reproduktion på 2009.</t>
+  </si>
+  <si>
+    <t>Lars skulle se vad han hade. Han har mailat en del data tidigare år (c:a 2000 - 2005)  till Tomas Meijer och kanske till Anders. Gick inte att få ut något vettigt ur databasen. Det fattas årtal och datum på majoriteten av lybesöken.</t>
+  </si>
+  <si>
+    <t>fått datan av Rasmus. Gjort en separat fil för de ripinventerade lyorna, dock verkar det saknas data för "2003", "2006", "2009", "2012", "2016". 2016 tog jag ur rovbase. 2012 var det inga. 2009 var det två. 2003 och 2006 finns i Peters fil (inlagt). Mailat Alva för att få ett utdrag ur databasen istället.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -160,6 +160,11 @@
       <color rgb="FF00B050"/>
       <name val="Calibri (Brödtext)_x0000_"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="Calibri (Brödtext)_x0000_"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -181,12 +186,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B3727A8-9212-7041-83C2-501947B2BAAE}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -572,7 +578,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -583,7 +589,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -594,7 +600,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -605,18 +611,18 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>7</v>
+      <c r="B11" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -627,7 +633,7 @@
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -662,32 +668,33 @@
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
matar in area i lydata sommar. Gjort en sammanställning över vilka lyor med kullar jag har. Skapat en shapefil med myrar för sverige.
</commit_message>
<xml_diff>
--- a/Rawdata/metadataframsteg.xlsx
+++ b/Rawdata/metadataframsteg.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-360" yWindow="5620" windowWidth="25440" windowHeight="11340" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
+    <workbookView xWindow="3580" yWindow="2400" windowWidth="25440" windowHeight="11340" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
   <si>
     <t>Moment</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>fått datan av Rasmus. Gjort en separat fil för de ripinventerade lyorna, dock verkar det saknas data för "2003", "2006", "2009", "2012", "2016". 2016 tog jag ur rovbase. 2012 var det inga. 2009 var det två. 2003 och 2006 finns i Peters fil (inlagt). Mailat Alva för att få ett utdrag ur databasen istället.</t>
+  </si>
+  <si>
+    <t>fattas endast area. Måste mäta sonden och skorna för att kunna lägga in.</t>
+  </si>
+  <si>
+    <t>har än så länge bara fångstdata med lyprecision mellan 00 och 04.</t>
   </si>
 </sst>
 </file>
@@ -509,7 +515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B3727A8-9212-7041-83C2-501947B2BAAE}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -542,8 +548,8 @@
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -558,8 +564,11 @@
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -650,6 +659,9 @@
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" customHeight="1">

</xml_diff>

<commit_message>
lagt in lyornas area.
</commit_message>
<xml_diff>
--- a/Rawdata/metadataframsteg.xlsx
+++ b/Rawdata/metadataframsteg.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="2400" windowWidth="25440" windowHeight="11340" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
+    <workbookView xWindow="160" yWindow="2400" windowWidth="25440" windowHeight="11340" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>Moment</t>
   </si>
@@ -120,9 +120,6 @@
   </si>
   <si>
     <t>fått datan av Rasmus. Gjort en separat fil för de ripinventerade lyorna, dock verkar det saknas data för "2003", "2006", "2009", "2012", "2016". 2016 tog jag ur rovbase. 2012 var det inga. 2009 var det två. 2003 och 2006 finns i Peters fil (inlagt). Mailat Alva för att få ett utdrag ur databasen istället.</t>
-  </si>
-  <si>
-    <t>fattas endast area. Måste mäta sonden och skorna för att kunna lägga in.</t>
   </si>
   <si>
     <t>har än så länge bara fångstdata med lyprecision mellan 00 och 04.</t>
@@ -516,7 +513,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -564,11 +561,8 @@
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
+      <c r="B5" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -661,7 +655,7 @@
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" customHeight="1">

</xml_diff>

<commit_message>
avtstånd närmsta föryngring klart.
</commit_message>
<xml_diff>
--- a/Rawdata/metadataframsteg.xlsx
+++ b/Rawdata/metadataframsteg.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="160" yWindow="2400" windowWidth="25440" windowHeight="11340" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
+    <workbookView xWindow="160" yWindow="3200" windowWidth="25440" windowHeight="11340" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -113,9 +113,6 @@
     <t>Den högsta sannolikheten för lämmel i en 500 x 500 m pixel är 0,4 under ett uppgångsår. Jag räknar allt från 0,2 och över som bra lämmelhabitat. Toppåren är inte lika intressanta eftersom lämlarna finns överallt.</t>
   </si>
   <si>
-    <t>Fått skript av Rasmus, ändra om till mina data. Fattas för vissa år i Rasmus.kulldata till Tor och i Lypositioner kullar 2000-2017 SWEREF99 per kull (finns mer data i den senare även fast Rasmus tagit bort lågår och omatade lyor. Komplettera med data från filen Red fox feeding och hitta vilka två lyor det var reproduktion på 2009.</t>
-  </si>
-  <si>
     <t>Lars skulle se vad han hade. Han har mailat en del data tidigare år (c:a 2000 - 2005)  till Tomas Meijer och kanske till Anders. Gick inte att få ut något vettigt ur databasen. Det fattas årtal och datum på majoriteten av lybesöken.</t>
   </si>
   <si>
@@ -123,13 +120,16 @@
   </si>
   <si>
     <t>har än så länge bara fångstdata med lyprecision mellan 00 och 04.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jag borde ha alla avstånd nu. Det kan hända att jag har något avstånd för mycket ifall det visar sig att en viss lya inte hade kull. Gör om i så fall. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -163,11 +163,6 @@
       <color rgb="FF00B050"/>
       <name val="Calibri (Brödtext)_x0000_"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="8" tint="-0.249977111117893"/>
-      <name val="Calibri (Brödtext)_x0000_"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -189,13 +184,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,7 +507,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -581,7 +575,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -592,7 +586,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -621,11 +615,11 @@
       <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>6</v>
+      <c r="B11" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -655,7 +649,7 @@
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" customHeight="1">

</xml_diff>

<commit_message>
Färdigt skript för andel vatten och myr runt lyor (gjorde det största jobbet i qgis). Påbörjad metoddel och uppdaterat framsteg.
</commit_message>
<xml_diff>
--- a/Rawdata/metadataframsteg.xlsx
+++ b/Rawdata/metadataframsteg.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-6240" yWindow="680" windowWidth="26860" windowHeight="12140" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
+    <workbookView xWindow="1500" yWindow="1820" windowWidth="25600" windowHeight="12140" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>Moment</t>
   </si>
@@ -65,9 +65,6 @@
     <t>GIS-data lyornas höjd över havet</t>
   </si>
   <si>
-    <t xml:space="preserve">GIS-data lyornas avstånd vattendrag eller sjöar </t>
-  </si>
-  <si>
     <t>GIS-data lyornas avstånd trädgräns</t>
   </si>
   <si>
@@ -89,21 +86,12 @@
     <t>Behöver jag den här? Kanske onödig. Får se vad NDVI säger först.</t>
   </si>
   <si>
-    <t>Sannolikhet för lämmel inom riptriangeln runt lyan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">iptrianglarna eftersom rävar jagar närmare lyan när de har valpar (Frafjord 1993) och måste bära tillbaka mat till lyan (Zapata et al. 1998. Dessutom måste jag hålla observationerna oberoende av varandra. Gallant et al (2014) valde max radius på 1,5 km. </t>
-  </si>
-  <si>
     <t>Andel bra lämmelhabitat inom området (sätt gränsvärde för lämmelsannolikhet per pixel)</t>
   </si>
   <si>
     <t>tog bort små trädsamlingar som inte satt ihop med skog som går ner i låglandet.</t>
   </si>
   <si>
-    <t>klart för de ripinventerade lyorna, klart för närmsta vattenkälla för alla lyor. Måste ta avstånd till större vatten. Bestäm ett gränsvärde (m^2), lägg till i attributes och ta bort.</t>
-  </si>
-  <si>
     <t>Den högsta sannolikheten för lämmel i en 500 x 500 m pixel är 0,4 under ett uppgångsår. Jag räknar allt från 0,2 och över som bra lämmelhabitat. Toppåren är inte lika intressanta eftersom lämlarna finns överallt.</t>
   </si>
   <si>
@@ -113,29 +101,44 @@
     <t xml:space="preserve"> Gjort en sammanställning av kullar från fyra filer: "komplexa kullar Helags - genetiskt och observationer.csv"som har en sammanställning fram till 2017, Helags_Red_Fox_Feeding (från Peter, uppdaterad till 2008), BEBODDA_LYOR_HEF 00_10 (uppdaterad till 2010) och Fjellområder_kull_1977_2016_Bodil_Nina (som bara innehåller antalet kullar, inte specifika lyor. De stämmer inte överens med varandra. Sammanställningen heter "min sammanställning plus BEBODDA_LYOR_HEF 00_10.xlsx". Mailat Alva för att få ett utdrag ur databasen istället.</t>
   </si>
   <si>
-    <t>GIS-data avstånd myrar</t>
-  </si>
-  <si>
-    <t>kanske borde ha med myrar (vadare). Har en shapefil med myrar på svenska sidan.</t>
-  </si>
-  <si>
     <t>GIS-data reproduktiva lyors avstånd till andra reprod. lyor</t>
   </si>
   <si>
-    <t>Lars skulle se vad han hade. Han har mailat en del data tidigare år (c:a 2000 - 2005)  till Tomas Meijer och kanske till Anders. Alva kunde inte få ut något vettigt ur databasen. Det fattas årtal och datum på majoriteten av lybesöken. Det jag har nu är vinteraktivitet mellan 2000 och 2001 (BEBODDA_LYOR_HEF 00_10).</t>
-  </si>
-  <si>
     <t xml:space="preserve">det finns rödrävsreproduktion i Peters fil fram till 2008 (röd text) dock är det bara två totalt. Använd koordinaterna för skjutna rävar istället. Finns fram till 2012 i Peters fil (Helags_Red_Fox_Feeding).  Använd Rasmus skript. </t>
   </si>
   <si>
     <t>har än så länge bara fångstdata med lyprecision mellan 01 och 04 (Gnagfånst 2001-04 2004-09-16) och 08 och 14 (Sammanfattning08-14.xlsx). Mailat Malin Larm om gnagardata 2015 -2017. Saknas alltså 2005 - 2007. Rasmus tror att datan för de åren kan ha dålig kvalitet.</t>
+  </si>
+  <si>
+    <t>Lars skulle se vad han hade. Han har mailat en del data tidigare år (c:a 2000 - 2005)  till Tomas Meijer och kanske till Anders. Alva kunde inte få ut något vettigt ur databasen. Det fattas årtal och datum på majoriteten av lybesöken. Det jag har nu är vinteraktivitet mellan 2000 och 2010 (BEBODDA_LYOR_HEF 00_10).</t>
+  </si>
+  <si>
+    <t>Myrar (vadare och lämmel). Tar andel myr inom en radie på 1,5 km (samma avstånd som Gallant et al 2014 gjorde för sina parametrar). Tar cirkel, inte triangel.</t>
+  </si>
+  <si>
+    <t>GIS-data area myrar inom 1,5 km radie</t>
+  </si>
+  <si>
+    <t>GIS-data lyornas avstånd vatten, area vatten inom 1,5 km radie</t>
+  </si>
+  <si>
+    <t>Klart för närmsta vattenkälla för alla lyor. Tog andel vatten inom 1,5 km radie istället för närmsta avstånd till större vatten.</t>
+  </si>
+  <si>
+    <t>på flera ripobsar ligger flera ripor på samma rad med samma gps -punkt, vinkel och avstånd. Detta måste ändras så att alla individer har en egen rad. Miss av mig att inte ta vinkel och avstånd till alla ripor.</t>
+  </si>
+  <si>
+    <t>Sannolikhet för lämmel inom 1,5 km runt lyan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,5 km eftersom rävar jagar närmare lyan när de har valpar (Frafjord 1993) och måste bära tillbaka mat till lyan (Zapata et al. 1998. Det är vettigare att ta en cirkelradie än riptrianglarna. Dessutom måste jag hålla observationerna oberoende av varandra. Gallant et al (2014) valde max radius på 1,5 km. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -169,6 +172,11 @@
       <color rgb="FF00B050"/>
       <name val="Calibri (Brödtext)_x0000_"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Calibri (Brödtext)_x0000_"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -190,12 +198,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,7 +522,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -540,6 +549,9 @@
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
@@ -575,13 +587,13 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -592,62 +604,62 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>6</v>
+        <v>31</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
         <v>29</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -660,18 +672,18 @@
     </row>
     <row r="15" spans="1:3" ht="15" customHeight="1">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
@@ -679,35 +691,35 @@
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hittat några år med fågeldata. Fått fram medelvärde för lämmel runt lyor. Försöker få fram andel bra lyhabitat. Känns som att jag har för många pixlar per buffer. Pixlarna är 500 X 500 m så borde vara färre.
</commit_message>
<xml_diff>
--- a/Rawdata/metadataframsteg.xlsx
+++ b/Rawdata/metadataframsteg.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1820" windowWidth="25600" windowHeight="12140" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
+    <workbookView xWindow="0" yWindow="1820" windowWidth="25600" windowHeight="12140" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t>Moment</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t xml:space="preserve">1,5 km eftersom rävar jagar närmare lyan när de har valpar (Frafjord 1993) och måste bära tillbaka mat till lyan (Zapata et al. 1998. Det är vettigare att ta en cirkelradie än riptrianglarna. Dessutom måste jag hålla observationerna oberoende av varandra. Gallant et al (2014) valde max radius på 1,5 km. </t>
+  </si>
+  <si>
+    <t>Distance sampling-analys på ripdata</t>
   </si>
 </sst>
 </file>
@@ -519,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B3727A8-9212-7041-83C2-501947B2BAAE}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -579,146 +582,154 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>2</v>
+        <v>36</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1">
-      <c r="A15" t="s">
+      <c r="B15" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15" customHeight="1">
+      <c r="A16" t="s">
         <v>15</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1">
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+    </row>
+    <row r="18" spans="1:3" ht="15" customHeight="1">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Lagt till myr och lybuffer shapefiler. Skript lämmelsannolikhet runt lyor. Skrivit metod
</commit_message>
<xml_diff>
--- a/Rawdata/metadataframsteg.xlsx
+++ b/Rawdata/metadataframsteg.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1820" windowWidth="25600" windowHeight="12140" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="25600" windowHeight="12140" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
   <si>
     <t>Moment</t>
   </si>
@@ -104,15 +104,6 @@
     <t>GIS-data reproduktiva lyors avstånd till andra reprod. lyor</t>
   </si>
   <si>
-    <t xml:space="preserve">det finns rödrävsreproduktion i Peters fil fram till 2008 (röd text) dock är det bara två totalt. Använd koordinaterna för skjutna rävar istället. Finns fram till 2012 i Peters fil (Helags_Red_Fox_Feeding).  Använd Rasmus skript. </t>
-  </si>
-  <si>
-    <t>har än så länge bara fångstdata med lyprecision mellan 01 och 04 (Gnagfånst 2001-04 2004-09-16) och 08 och 14 (Sammanfattning08-14.xlsx). Mailat Malin Larm om gnagardata 2015 -2017. Saknas alltså 2005 - 2007. Rasmus tror att datan för de åren kan ha dålig kvalitet.</t>
-  </si>
-  <si>
-    <t>Lars skulle se vad han hade. Han har mailat en del data tidigare år (c:a 2000 - 2005)  till Tomas Meijer och kanske till Anders. Alva kunde inte få ut något vettigt ur databasen. Det fattas årtal och datum på majoriteten av lybesöken. Det jag har nu är vinteraktivitet mellan 2000 och 2010 (BEBODDA_LYOR_HEF 00_10).</t>
-  </si>
-  <si>
     <t>Myrar (vadare och lämmel). Tar andel myr inom en radie på 1,5 km (samma avstånd som Gallant et al 2014 gjorde för sina parametrar). Tar cirkel, inte triangel.</t>
   </si>
   <si>
@@ -131,10 +122,22 @@
     <t>Sannolikhet för lämmel inom 1,5 km runt lyan</t>
   </si>
   <si>
-    <t xml:space="preserve">1,5 km eftersom rävar jagar närmare lyan när de har valpar (Frafjord 1993) och måste bära tillbaka mat till lyan (Zapata et al. 1998. Det är vettigare att ta en cirkelradie än riptrianglarna. Dessutom måste jag hålla observationerna oberoende av varandra. Gallant et al (2014) valde max radius på 1,5 km. </t>
-  </si>
-  <si>
     <t>Distance sampling-analys på ripdata</t>
+  </si>
+  <si>
+    <t>Saknar vinter/våraktivitet mellan 2011 och 2014. Har bara vinteraktivitet mellan 2000 och 2011 (vet ej vilka exakta datum).  Lars har mailat en del data tidigare år (c:a 2000 - 2005)  till Tomas Meijer och kanske till Anders. Alva kunde inte få ut något vettigt ur databasen. Det fattas årtal och datum på majoriteten av lybesöken. Det jag har nu är vinteraktivitet mellan 2000 och 2010 (BEBODDA_LYOR_HEF 00_10).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">det finns rödrävsreproduktion i Peters fil fram till 2008 (röd text) dock är det bara två totalt. Använd koordinaterna för skjutna rävar istället. Finns fram till 2012 i Peters fil.  (Helags_Red_Fox_Feeding).  Maila Lars om resten. Använd Rasmus skript. </t>
+  </si>
+  <si>
+    <t>har mellan 2005 och 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klar men pixlarna är endast 49 * 43 m. Inte 500 * 500 meter. 1,5 km eftersom rävar jagar närmare lyan när de har valpar (Frafjord 1993) och måste bära tillbaka mat till lyan (Zapata et al. 1998. Det är vettigare att ta en cirkelradie än riptrianglarna. Dessutom måste jag hålla observationerna oberoende av varandra. Gallant et al (2014) valde max radius på 1,5 km. </t>
+  </si>
+  <si>
+    <t>Fångstdatan ingår ju i lämmelmodellen så kanske är onödigt? har än så länge bara fångstdata med lyprecision mellan 01 och 04 (Gnagfånst 2001-04 2004-09-16) och 08 och 14 (Sammanfattning08-14.xlsx). Mailat Malin Larm om gnagardata 2015 -2017. Saknas alltså 2005 - 2007. Rasmus tror att datan för de åren kan ha dålig kvalitet.</t>
   </si>
 </sst>
 </file>
@@ -525,7 +528,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -553,7 +556,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -582,7 +585,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
@@ -604,7 +607,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -631,24 +634,24 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -670,7 +673,7 @@
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -685,19 +688,22 @@
       <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>7</v>
+      <c r="B16" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>7</v>
+      <c r="B17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1">
@@ -713,21 +719,21 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>7</v>
+        <v>31</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>7</v>
+      <c r="B20" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="C20" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Lagt till rader för riptransekter där det var dubbla obsar. uppdaterat framsteg. gjort skript och printat ut en fil med lämmelsannolikheter.gjort filer för att skicka till Lars. Gjort skript och printat fil med andel lämmelhabitattyper per lya. KOmmer en till sådan med annan metod för att klassificera bra och dåliga lyor.
</commit_message>
<xml_diff>
--- a/Rawdata/metadataframsteg.xlsx
+++ b/Rawdata/metadataframsteg.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="25600" windowHeight="12140" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
+    <workbookView xWindow="420" yWindow="1840" windowWidth="25600" windowHeight="12140" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -92,15 +92,9 @@
     <t>tog bort små trädsamlingar som inte satt ihop med skog som går ner i låglandet.</t>
   </si>
   <si>
-    <t>Den högsta sannolikheten för lämmel i en 500 x 500 m pixel är 0,4 under ett uppgångsår. Jag räknar allt från 0,2 och över som bra lämmelhabitat. Toppåren är inte lika intressanta eftersom lämlarna finns överallt.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Jag borde ha alla avstånd nu. Det kan hända att jag har något avstånd för mycket ifall det visar sig att en viss lya inte hade kull. Gör om i så fall. </t>
   </si>
   <si>
-    <t xml:space="preserve"> Gjort en sammanställning av kullar från fyra filer: "komplexa kullar Helags - genetiskt och observationer.csv"som har en sammanställning fram till 2017, Helags_Red_Fox_Feeding (från Peter, uppdaterad till 2008), BEBODDA_LYOR_HEF 00_10 (uppdaterad till 2010) och Fjellområder_kull_1977_2016_Bodil_Nina (som bara innehåller antalet kullar, inte specifika lyor. De stämmer inte överens med varandra. Sammanställningen heter "min sammanställning plus BEBODDA_LYOR_HEF 00_10.xlsx". Mailat Alva för att få ett utdrag ur databasen istället.</t>
-  </si>
-  <si>
     <t>GIS-data reproduktiva lyors avstånd till andra reprod. lyor</t>
   </si>
   <si>
@@ -125,19 +119,25 @@
     <t>Distance sampling-analys på ripdata</t>
   </si>
   <si>
-    <t>Saknar vinter/våraktivitet mellan 2011 och 2014. Har bara vinteraktivitet mellan 2000 och 2011 (vet ej vilka exakta datum).  Lars har mailat en del data tidigare år (c:a 2000 - 2005)  till Tomas Meijer och kanske till Anders. Alva kunde inte få ut något vettigt ur databasen. Det fattas årtal och datum på majoriteten av lybesöken. Det jag har nu är vinteraktivitet mellan 2000 och 2010 (BEBODDA_LYOR_HEF 00_10).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">det finns rödrävsreproduktion i Peters fil fram till 2008 (röd text) dock är det bara två totalt. Använd koordinaterna för skjutna rävar istället. Finns fram till 2012 i Peters fil.  (Helags_Red_Fox_Feeding).  Maila Lars om resten. Använd Rasmus skript. </t>
-  </si>
-  <si>
-    <t>har mellan 2005 och 2008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Klar men pixlarna är endast 49 * 43 m. Inte 500 * 500 meter. 1,5 km eftersom rävar jagar närmare lyan när de har valpar (Frafjord 1993) och måste bära tillbaka mat till lyan (Zapata et al. 1998. Det är vettigare att ta en cirkelradie än riptrianglarna. Dessutom måste jag hålla observationerna oberoende av varandra. Gallant et al (2014) valde max radius på 1,5 km. </t>
-  </si>
-  <si>
-    <t>Fångstdatan ingår ju i lämmelmodellen så kanske är onödigt? har än så länge bara fångstdata med lyprecision mellan 01 och 04 (Gnagfånst 2001-04 2004-09-16) och 08 och 14 (Sammanfattning08-14.xlsx). Mailat Malin Larm om gnagardata 2015 -2017. Saknas alltså 2005 - 2007. Rasmus tror att datan för de åren kan ha dålig kvalitet.</t>
+    <t>Saknar vinter/våraktivitet mellan 2011 och 2014. Har bara vinteraktivitet mellan 2000 och 2011 (vet ej vilka exakta datum). Har mailat Lars om 2011 -2014. Lars har mailat en del data tidigare år (c:a 2000 - 2005)  till Tomas Meijer och kanske till Anders. Alva kunde inte få ut något vettigt ur databasen. Det fattas årtal och datum på majoriteten av lybesöken. Det jag har nu är vinteraktivitet mellan 2000 och 2010 (BEBODDA_LYOR_HEF 00_10).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">det finns rödrävsreproduktion i Peters fil fram till 2008 (röd text) dock är det bara två totalt. Använd koordinaterna för skjutna rävar istället. Finns fram till 2012 i Peters fil. (Helags_Red_Fox_Feeding).  Mailat Lars om resten. Använd Rasmus skript. </t>
+  </si>
+  <si>
+    <t>har mellan 2005 och 2008. Fick fler år av Karin också. Gå igenom.</t>
+  </si>
+  <si>
+    <t>Ingår fångstdatan i rastern jag fick av Rasmus? har fångstdata med lyprecision mellan 01 och 04 (Gnagfånst 2001-04 2004-09-16) och 08 och 14 (Sammanfattning08-14.xlsx). Fick en fil av Malin Larm om med en sammanfattning av gnagare 2008 -2017. 2009 och 2016 är dock inte med. Saknas alltså 2005 - 2007. Rasmus tror att datan för de åren kan ha dålig kvalitet. Fick en fil av Karin (Gnagarfångst2007) men den verkar bara ha för vindelfjällen för 2007.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1,5 km eftersom rävar jagar närmare lyan när de har valpar (Frafjord 1993) och måste bära tillbaka mat till lyan (Zapata et al. 1998. Det är vettigare att ta en cirkelradie än riptrianglarna. Dessutom måste jag hålla observationerna oberoende av varandra. Gallant et al (2014) valde max radius på 1,5 km. </t>
+  </si>
+  <si>
+    <t>Den högsta medelvärdessannolikheten för lämmel i en lybuffer  är 0,53 under ett uppgångsår. Jag räknar allt från 0,265 och över som bra lämmelhabitat.  Medelbra är satt mellan 0,265 och medianen för medelvärdessannolikheten för lämmel i en lybuffer. Under medianen är dåliga  lämmelhabitat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gjort en sammanställning av kullar från fyra filer: "komplexa kullar Helags - genetiskt och observationer.csv"som har en sammanställning fram till 2017, Helags_Red_Fox_Feeding (från Peter, uppdaterad till 2008), BEBODDA_LYOR_HEF 00_10 (uppdaterad till 2010) och Fjellområder_kull_1977_2016_Bodil_Nina (som bara innehåller antalet kullar, inte specifika lyor. De stämmer inte överens med varandra. Sammanställningen heter "min sammanställning plus BEBODDA_LYOR_HEF 00_10.xlsx". Mailat Alva för att få ett utdrag ur databasen istället. Fick en ny fil av Bodil men den hjälpte inte. Typ som som Fjellområder_kull-filen.</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C12" sqref="C12:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -556,7 +556,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -585,7 +585,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
@@ -607,7 +607,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -618,7 +618,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -634,35 +634,35 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -673,7 +673,7 @@
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -692,7 +692,7 @@
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -703,7 +703,7 @@
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1">
@@ -719,24 +719,24 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>6</v>
+      <c r="B20" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gör distance function för riporna. la till lite anteckningar i städar rödrävsdata. Printat en excelfil med ripor för att lägga till väderklassificeringar manuellt.
</commit_message>
<xml_diff>
--- a/Rawdata/metadataframsteg.xlsx
+++ b/Rawdata/metadataframsteg.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="420" yWindow="1840" windowWidth="25600" windowHeight="12140" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
+    <workbookView xWindow="2600" yWindow="1840" windowWidth="25600" windowHeight="12140" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
   <si>
     <t>Moment</t>
   </si>
@@ -89,27 +89,18 @@
     <t>Andel bra lämmelhabitat inom området (sätt gränsvärde för lämmelsannolikhet per pixel)</t>
   </si>
   <si>
-    <t>tog bort små trädsamlingar som inte satt ihop med skog som går ner i låglandet.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Jag borde ha alla avstånd nu. Det kan hända att jag har något avstånd för mycket ifall det visar sig att en viss lya inte hade kull. Gör om i så fall. </t>
   </si>
   <si>
     <t>GIS-data reproduktiva lyors avstånd till andra reprod. lyor</t>
   </si>
   <si>
-    <t>Myrar (vadare och lämmel). Tar andel myr inom en radie på 1,5 km (samma avstånd som Gallant et al 2014 gjorde för sina parametrar). Tar cirkel, inte triangel.</t>
-  </si>
-  <si>
     <t>GIS-data area myrar inom 1,5 km radie</t>
   </si>
   <si>
     <t>GIS-data lyornas avstånd vatten, area vatten inom 1,5 km radie</t>
   </si>
   <si>
-    <t>Klart för närmsta vattenkälla för alla lyor. Tog andel vatten inom 1,5 km radie istället för närmsta avstånd till större vatten.</t>
-  </si>
-  <si>
     <t>på flera ripobsar ligger flera ripor på samma rad med samma gps -punkt, vinkel och avstånd. Detta måste ändras så att alla individer har en egen rad. Miss av mig att inte ta vinkel och avstånd till alla ripor.</t>
   </si>
   <si>
@@ -119,32 +110,59 @@
     <t>Distance sampling-analys på ripdata</t>
   </si>
   <si>
-    <t>Saknar vinter/våraktivitet mellan 2011 och 2014. Har bara vinteraktivitet mellan 2000 och 2011 (vet ej vilka exakta datum). Har mailat Lars om 2011 -2014. Lars har mailat en del data tidigare år (c:a 2000 - 2005)  till Tomas Meijer och kanske till Anders. Alva kunde inte få ut något vettigt ur databasen. Det fattas årtal och datum på majoriteten av lybesöken. Det jag har nu är vinteraktivitet mellan 2000 och 2010 (BEBODDA_LYOR_HEF 00_10).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">det finns rödrävsreproduktion i Peters fil fram till 2008 (röd text) dock är det bara två totalt. Använd koordinaterna för skjutna rävar istället. Finns fram till 2012 i Peters fil. (Helags_Red_Fox_Feeding).  Mailat Lars om resten. Använd Rasmus skript. </t>
-  </si>
-  <si>
     <t>har mellan 2005 och 2008. Fick fler år av Karin också. Gå igenom.</t>
   </si>
   <si>
     <t>Ingår fångstdatan i rastern jag fick av Rasmus? har fångstdata med lyprecision mellan 01 och 04 (Gnagfånst 2001-04 2004-09-16) och 08 och 14 (Sammanfattning08-14.xlsx). Fick en fil av Malin Larm om med en sammanfattning av gnagare 2008 -2017. 2009 och 2016 är dock inte med. Saknas alltså 2005 - 2007. Rasmus tror att datan för de åren kan ha dålig kvalitet. Fick en fil av Karin (Gnagarfångst2007) men den verkar bara ha för vindelfjällen för 2007.</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1,5 km eftersom rävar jagar närmare lyan när de har valpar (Frafjord 1993) och måste bära tillbaka mat till lyan (Zapata et al. 1998. Det är vettigare att ta en cirkelradie än riptrianglarna. Dessutom måste jag hålla observationerna oberoende av varandra. Gallant et al (2014) valde max radius på 1,5 km. </t>
-  </si>
-  <si>
-    <t>Den högsta medelvärdessannolikheten för lämmel i en lybuffer  är 0,53 under ett uppgångsår. Jag räknar allt från 0,265 och över som bra lämmelhabitat.  Medelbra är satt mellan 0,265 och medianen för medelvärdessannolikheten för lämmel i en lybuffer. Under medianen är dåliga  lämmelhabitat.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Gjort en sammanställning av kullar från fyra filer: "komplexa kullar Helags - genetiskt och observationer.csv"som har en sammanställning fram till 2017, Helags_Red_Fox_Feeding (från Peter, uppdaterad till 2008), BEBODDA_LYOR_HEF 00_10 (uppdaterad till 2010) och Fjellområder_kull_1977_2016_Bodil_Nina (som bara innehåller antalet kullar, inte specifika lyor. De stämmer inte överens med varandra. Sammanställningen heter "min sammanställning plus BEBODDA_LYOR_HEF 00_10.xlsx". Mailat Alva för att få ett utdrag ur databasen istället. Fick en ny fil av Bodil men den hjälpte inte. Typ som som Fjellområder_kull-filen.</t>
+  </si>
+  <si>
+    <t>avvaktar</t>
+  </si>
+  <si>
+    <t>KOLLA SÅ ATT ALLT ÄR I EPSG:3006 Sweref! tog bort små trädsamlingar som inte satt ihop med skog som går ner i låglandet.</t>
+  </si>
+  <si>
+    <t>KOLLA SÅ ATT ALLT ÄR I EPSG:3006 Sweref! Klart för närmsta vattenkälla för alla lyor. Tog andel vatten inom 1,5 km radie istället för närmsta avstånd till större vatten.</t>
+  </si>
+  <si>
+    <t>KOLLA SÅ ATT ALLT ÄR I EPSG:3006 Sweref! Myrar (vadare och lämmel). Tar andel myr inom en radie på 1,5 km (samma avstånd som Gallant et al 2014 gjorde för sina parametrar). KOLLA SÅ ATT ALLT ÄR I EPSG:3006 Sweref! Tar cirkel, inte triangel.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> KOLLA SÅ ATT ALLT ÄR I EPSG:3006 Sweref! 1,5 km eftersom rävar jagar närmare lyan när de har valpar (Frafjord 1993) och måste bära tillbaka mat till lyan (Zapata et al. 1998. Det är vettigare att ta en cirkelradie än riptrianglarna. Dessutom måste jag hålla observationerna oberoende av varandra. Gallant et al (2014) valde max radius på 1,5 km. </t>
+  </si>
+  <si>
+    <t>KOLLA SÅ ATT ALLT ÄR I EPSG:3006 Sweref! Den högsta medelvärdessannolikheten för lämmel i en lybuffer  är 0,53 under ett uppgångsår. Jag räknar allt från 0,265 och över som bra lämmelhabitat.  Medelbra är satt mellan 0,265 och medianen för medelvärdessannolikheten för lämmel i en lybuffer. Under medianen är dåliga  lämmelhabitat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gjort shapefil och excel fil i EPSG:3006 sweref med skjutna rödrävar mellan 2000 och 2016 från Peters och Lars filer. Finns för de två senaste vintrarna på rovbasen. limma in i excel därifrån. det finns rödrävsreproduktion i Peters fil fram till 2008 (röd text) dock är det bara två totalt. Använd Rasmus skript. </t>
+  </si>
+  <si>
+    <t>AIC</t>
+  </si>
+  <si>
+    <t>Metod</t>
+  </si>
+  <si>
+    <t>Inledning</t>
+  </si>
+  <si>
+    <t>Resultat</t>
+  </si>
+  <si>
+    <t>Diskussion</t>
+  </si>
+  <si>
+    <t>Se Karins mail för relativ aktivitet.Saknar vinter/våraktivitet mellan 2011 och 2014. Har bara vinteraktivitet mellan 2000 och 2011 (vet ej vilka exakta datum). Har mailat Lars om 2011 -2014. Lars har mailat en del data tidigare år (c:a 2000 - 2005)  till Tomas Meijer och kanske till Anders. Alva kunde inte få ut något vettigt ur databasen. Det fattas årtal och datum på majoriteten av lybesöken. Det jag har nu är vinteraktivitet mellan 2000 och 2010 (BEBODDA_LYOR_HEF 00_10).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -183,6 +201,17 @@
       <color theme="9"/>
       <name val="Calibri (Brödtext)_x0000_"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Brödtext)_x0000_"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri (Brödtext)_x0000_"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -204,13 +233,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B3727A8-9212-7041-83C2-501947B2BAAE}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:C13"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -556,7 +587,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -585,7 +616,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
@@ -607,7 +638,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -618,7 +649,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -629,51 +660,51 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>7</v>
+      <c r="B14" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -688,30 +719,30 @@
       <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>6</v>
+      <c r="B16" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>6</v>
+      <c r="B17" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1">
       <c r="A18" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>7</v>
+      <c r="B18" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="C18" t="s">
         <v>19</v>
@@ -719,7 +750,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>2</v>
@@ -737,6 +768,46 @@
       </c>
       <c r="C20" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Har räknat ut hur många gånger det har varit kull per lya mellan 2000 och 2018. Har även räknat ut hur många gånger lyorna inventerats mellan 2000-2010 och mellan 2015-2018. Uppdaterat metadataframsteg
</commit_message>
<xml_diff>
--- a/Rawdata/metadataframsteg.xlsx
+++ b/Rawdata/metadataframsteg.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4840" yWindow="700" windowWidth="25600" windowHeight="12140" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
+    <workbookView xWindow="1620" yWindow="1220" windowWidth="25600" windowHeight="12140" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="52">
   <si>
     <t>Moment</t>
   </si>
@@ -125,12 +125,6 @@
     <t>KOLLA SÅ ATT ALLT ÄR I EPSG:3006 Sweref! Den högsta medelvärdessannolikheten för lämmel i en lybuffer  är 0,53 under ett uppgångsår. Jag räknar allt från 0,265 och över som bra lämmelhabitat.  Medelbra är satt mellan 0,265 och medianen för medelvärdessannolikheten för lämmel i en lybuffer. Under medianen är dåliga  lämmelhabitat.</t>
   </si>
   <si>
-    <t xml:space="preserve">Gjort shapefil och excel fil i EPSG:3006 sweref med skjutna rödrävar mellan 2000 och 2016 från Peters och Lars filer. Finns för de två senaste vintrarna på rovbasen. limma in i excel därifrån. det finns rödrävsreproduktion i Peters fil fram till 2008 (röd text) dock är det bara två totalt. Använd Rasmus skript. </t>
-  </si>
-  <si>
-    <t>AIC</t>
-  </si>
-  <si>
     <t>Metod</t>
   </si>
   <si>
@@ -152,9 +146,6 @@
     <t>Blankan och Norr vaktklumpen klar. Myrar (vadare och lämmel). Tar andel myr inom en radie på 1,5 km (samma avstånd som Gallant et al 2014 gjorde för sina parametrar). KOLLA SÅ ATT ALLT ÄR I EPSG:3006 Sweref! Tar cirkel, inte triangel.</t>
   </si>
   <si>
-    <t>pen klar</t>
-  </si>
-  <si>
     <t>Blankan och Norr vaktklumpen klar</t>
   </si>
   <si>
@@ -165,6 +156,30 @@
   </si>
   <si>
     <t>Distance slutade krångla så nu är jag rätt nöjd. Dock är egentligen en mixture model bäst för ripspillningen men får inte ut spillning per lya</t>
+  </si>
+  <si>
+    <t>AIC  - skapa en fil med alla variabler för alla lyor</t>
+  </si>
+  <si>
+    <t>AIC  - skapa en fil med alla variabler för riplyor</t>
+  </si>
+  <si>
+    <t>Lyornas storlek</t>
+  </si>
+  <si>
+    <t>funkar ej</t>
+  </si>
+  <si>
+    <t>För svårt att se lyorna på IR-foto. Funkade inte ens att få hyfsat rätt på lyorna jag har mätt på riktigt. Skicka filen till Karin och Rasmus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gjort shapefil och excel fil i EPSG:3006 sweref med skjutna rödrävar mellan 2000 och 2016 från Peters och Lars filer. Finns för de två senaste vintrarna på rovbasen men kommer inte åt dem. limma in i excel därifrån. det finns rödrävsreproduktion i Peters fil fram till 2008 (röd text) dock är det bara två totalt. Använd Rasmus skript. </t>
+  </si>
+  <si>
+    <t>Relativt mått på kullar</t>
+  </si>
+  <si>
+    <t>Har räknat ut totala antalet kullar per lya. Har räknat ut antal inventeringar per lya mellan 2000 och 2010 (från BEBODDA_LYOR_HEF 00-10 ) och mellan 2015 och 2018 från en lista som jag plockade ut från rovbasen. Saknar alltså inventeringsdata på lyor mellan 2011 och 2014.</t>
   </si>
 </sst>
 </file>
@@ -565,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B3727A8-9212-7041-83C2-501947B2BAAE}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -577,7 +592,7 @@
     <col min="3" max="3" width="132.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -588,7 +603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -599,7 +614,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -607,7 +622,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -615,7 +630,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -623,7 +638,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -631,10 +646,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -642,7 +657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -650,10 +665,10 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -661,10 +676,10 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -672,10 +687,10 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -683,10 +698,10 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -694,10 +709,10 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -708,7 +723,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -716,10 +731,10 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -727,13 +742,10 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15" customHeight="1">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -790,31 +802,37 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>7</v>
+        <v>46</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="C22" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>6</v>
+        <v>44</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>7</v>
@@ -822,9 +840,33 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Gjort avstånd till rödräv mellan 2001 och 2015. Tog avstånd till lyorna sommaren innan de blev skjutna på vintern. Printat en fil. Pillat lite med AIC också men inte lagt till rödräv eller avstånd till reproduktiva fjällrävslyor.
</commit_message>
<xml_diff>
--- a/Rawdata/metadataframsteg.xlsx
+++ b/Rawdata/metadataframsteg.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="1220" windowWidth="25600" windowHeight="12140" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
+    <workbookView xWindow="0" yWindow="2780" windowWidth="25600" windowHeight="12140" xr2:uid="{33919143-3F5E-6040-9757-5DDE8D34639B}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -173,13 +173,13 @@
     <t>För svårt att se lyorna på IR-foto. Funkade inte ens att få hyfsat rätt på lyorna jag har mätt på riktigt. Skicka filen till Karin och Rasmus</t>
   </si>
   <si>
-    <t xml:space="preserve">Gjort shapefil och excel fil i EPSG:3006 sweref med skjutna rödrävar mellan 2000 och 2016 från Peters och Lars filer. Finns för de två senaste vintrarna på rovbasen men kommer inte åt dem. limma in i excel därifrån. det finns rödrävsreproduktion i Peters fil fram till 2008 (röd text) dock är det bara två totalt. Använd Rasmus skript. </t>
-  </si>
-  <si>
     <t>Relativt mått på kullar</t>
   </si>
   <si>
     <t>Har räknat ut totala antalet kullar per lya. Har räknat ut antal inventeringar per lya mellan 2000 och 2010 (från BEBODDA_LYOR_HEF 00-10 ) och mellan 2015 och 2018 från en lista som jag plockade ut från rovbasen. Saknar alltså inventeringsdata på lyor mellan 2011 och 2014.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Printat fil med avstånd år 2001 - 2015. Gjort shapefil och excel fil i EPSG:3006 sweref med skjutna rödrävar mellan 2000 och 2016 från Peters och Lars filer. Finns för de två senaste vintrarna på rovbasen men kommer inte åt dem. limma in i excel därifrån. det finns rödrävsreproduktion i Peters fil fram till 2008 (röd text) dock är det bara två totalt. Använd Rasmus skript. </t>
   </si>
 </sst>
 </file>
@@ -582,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B3727A8-9212-7041-83C2-501947B2BAAE}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -727,11 +727,11 @@
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>6</v>
+      <c r="B14" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -813,13 +813,13 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:3">

</xml_diff>